<commit_message>
fixed bug in cluster
</commit_message>
<xml_diff>
--- a/benchmarking/results/spot_llama-3-8b_ep10_training_ds_v16_3-17_1-2_lora_12052025_eval-summary.xlsx
+++ b/benchmarking/results/spot_llama-3-8b_ep10_training_ds_v16_3-17_1-2_lora_12052025_eval-summary.xlsx
@@ -663,10 +663,10 @@
         <v>0.8068181818181818</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9526515151515151</v>
+        <v>0.8882575757575758</v>
       </c>
       <c r="I2" t="n">
-        <v>0.8863636363636364</v>
+        <v>0.8882575757575758</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
@@ -675,13 +675,13 @@
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M2" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N2" t="n">
-        <v>0.6565656565656566</v>
+        <v>0.6161616161616161</v>
       </c>
       <c r="O2" t="n">
         <v>0.8333333333333334</v>
@@ -699,28 +699,28 @@
         <v>1</v>
       </c>
       <c r="T2" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U2" t="n">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="V2" t="n">
-        <v>0.7661016949152543</v>
+        <v>0.7627118644067796</v>
       </c>
       <c r="W2" t="n">
-        <v>0.7304347826086957</v>
+        <v>0.7260869565217392</v>
       </c>
       <c r="X2" t="n">
         <v>0.7230769230769231</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.7565217391304347</v>
+        <v>0.7521739130434782</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.7347826086956522</v>
+        <v>0.7304347826086957</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.7304347826086957</v>
+        <v>0.7260869565217392</v>
       </c>
       <c r="AB2" t="n">
         <v>0.6101694915254238</v>

</xml_diff>